<commit_message>
tweaks to country page formatting
</commit_message>
<xml_diff>
--- a/charts_download/explorers/health_metadata.xlsx
+++ b/charts_download/explorers/health_metadata.xlsx
@@ -30792,7 +30792,7 @@
         </is>
       </c>
       <c r="B1168" s="2" t="n">
-        <v>44855</v>
+        <v>44856</v>
       </c>
       <c r="C1168" t="inlineStr">
         <is>
@@ -30896,7 +30896,7 @@
         </is>
       </c>
       <c r="B1172" s="2" t="n">
-        <v>44854</v>
+        <v>44856</v>
       </c>
       <c r="C1172" t="inlineStr">
         <is>
@@ -31130,7 +31130,7 @@
         </is>
       </c>
       <c r="B1181" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1181" t="inlineStr">
         <is>
@@ -31312,7 +31312,7 @@
         </is>
       </c>
       <c r="B1188" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1188" t="inlineStr">
         <is>
@@ -31910,7 +31910,7 @@
         </is>
       </c>
       <c r="B1211" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1211" t="inlineStr">
         <is>
@@ -31936,7 +31936,7 @@
         </is>
       </c>
       <c r="B1212" s="2" t="n">
-        <v>44855</v>
+        <v>44857</v>
       </c>
       <c r="C1212" t="inlineStr">
         <is>
@@ -32040,7 +32040,7 @@
         </is>
       </c>
       <c r="B1216" s="2" t="n">
-        <v>44855</v>
+        <v>44856</v>
       </c>
       <c r="C1216" t="inlineStr">
         <is>
@@ -32612,7 +32612,7 @@
         </is>
       </c>
       <c r="B1238" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1238" t="inlineStr">
         <is>
@@ -32742,7 +32742,7 @@
         </is>
       </c>
       <c r="B1243" s="2" t="n">
-        <v>44850</v>
+        <v>44857</v>
       </c>
       <c r="C1243" t="inlineStr">
         <is>
@@ -32794,7 +32794,7 @@
         </is>
       </c>
       <c r="B1245" s="2" t="n">
-        <v>44854</v>
+        <v>44856</v>
       </c>
       <c r="C1245" t="inlineStr">
         <is>
@@ -32924,7 +32924,7 @@
         </is>
       </c>
       <c r="B1250" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1250" t="inlineStr">
         <is>
@@ -33054,7 +33054,7 @@
         </is>
       </c>
       <c r="B1255" s="2" t="n">
-        <v>44855</v>
+        <v>44857</v>
       </c>
       <c r="C1255" t="inlineStr">
         <is>
@@ -33080,7 +33080,7 @@
         </is>
       </c>
       <c r="B1256" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1256" t="inlineStr">
         <is>
@@ -33262,7 +33262,7 @@
         </is>
       </c>
       <c r="B1263" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1263" t="inlineStr">
         <is>
@@ -33366,7 +33366,7 @@
         </is>
       </c>
       <c r="B1267" s="2" t="n">
-        <v>44854</v>
+        <v>44857</v>
       </c>
       <c r="C1267" t="inlineStr">
         <is>
@@ -33938,7 +33938,7 @@
         </is>
       </c>
       <c r="B1289" s="2" t="n">
-        <v>44855</v>
+        <v>44856</v>
       </c>
       <c r="C1289" t="inlineStr">
         <is>
@@ -34172,7 +34172,7 @@
         </is>
       </c>
       <c r="B1298" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1298" t="inlineStr">
         <is>
@@ -34588,7 +34588,7 @@
         </is>
       </c>
       <c r="B1314" s="2" t="n">
-        <v>44849</v>
+        <v>44856</v>
       </c>
       <c r="C1314" t="inlineStr">
         <is>
@@ -34666,7 +34666,7 @@
         </is>
       </c>
       <c r="B1317" s="2" t="n">
-        <v>44855</v>
+        <v>44856</v>
       </c>
       <c r="C1317" t="inlineStr">
         <is>
@@ -35732,7 +35732,7 @@
         </is>
       </c>
       <c r="B1358" s="2" t="n">
-        <v>44856</v>
+        <v>44857</v>
       </c>
       <c r="C1358" t="inlineStr">
         <is>
@@ -35784,7 +35784,7 @@
         </is>
       </c>
       <c r="B1360" s="2" t="n">
-        <v>44855</v>
+        <v>44857</v>
       </c>
       <c r="C1360" t="inlineStr">
         <is>
@@ -36174,7 +36174,7 @@
         </is>
       </c>
       <c r="B1375" s="2" t="n">
-        <v>44855</v>
+        <v>44857</v>
       </c>
       <c r="C1375" t="inlineStr">
         <is>

</xml_diff>